<commit_message>
add password check with symbol
</commit_message>
<xml_diff>
--- a/doc/symbols.xlsx
+++ b/doc/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxikrause/VSCode/bambu-mqtt-pico/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7842E2F-57D9-5449-A2ED-9305710FB447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45E85A1-8083-DF48-8407-1B22D92C0FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{03AEDF40-5CD7-D34B-9CD6-B04860BB6D0B}"/>
   </bookViews>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7B81F8-BA37-E140-A257-454B71F67245}">
   <dimension ref="D3:AY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1438,16 +1438,16 @@
       <c r="E13" s="1">
         <v>62</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="4">
         <v>61</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="4">
         <v>60</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="4">
         <v>59</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="4">
         <v>58</v>
       </c>
       <c r="J13" s="1">
@@ -1560,7 +1560,7 @@
       <c r="E14" s="1">
         <v>54</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="4">
         <v>53</v>
       </c>
       <c r="G14" s="1">
@@ -1569,7 +1569,7 @@
       <c r="H14" s="1">
         <v>51</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="4">
         <v>50</v>
       </c>
       <c r="J14" s="1">
@@ -1682,7 +1682,7 @@
       <c r="E15" s="1">
         <v>46</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="4">
         <v>45</v>
       </c>
       <c r="G15" s="1">
@@ -1691,7 +1691,7 @@
       <c r="H15" s="1">
         <v>43</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="4">
         <v>42</v>
       </c>
       <c r="J15" s="1">
@@ -1801,22 +1801,22 @@
       <c r="D16" s="1">
         <v>39</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>38</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="4">
         <v>37</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="4">
         <v>36</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>35</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="4">
         <v>34</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="4">
         <v>33</v>
       </c>
       <c r="K16" s="1">
@@ -1923,22 +1923,22 @@
       <c r="D17" s="1">
         <v>31</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>30</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="4">
         <v>29</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="4">
         <v>28</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="4">
         <v>27</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="4">
         <v>26</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="4">
         <v>25</v>
       </c>
       <c r="K17" s="1">
@@ -2045,22 +2045,22 @@
       <c r="D18" s="1">
         <v>23</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>22</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="4">
         <v>21</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="4">
         <v>20</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="4">
         <v>19</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="4">
         <v>18</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="4">
         <v>17</v>
       </c>
       <c r="K18" s="1">
@@ -2167,22 +2167,22 @@
       <c r="D19" s="1">
         <v>15</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="4">
         <v>14</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="4">
         <v>13</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="4">
         <v>12</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="4">
         <v>11</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="4">
         <v>10</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="4">
         <v>9</v>
       </c>
       <c r="K19" s="1">
@@ -2289,22 +2289,22 @@
       <c r="D20" s="1">
         <v>7</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="4">
         <v>6</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="4">
         <v>5</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="4">
         <v>4</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="4">
         <v>3</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="4">
         <v>2</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="4">
         <v>1</v>
       </c>
       <c r="K20" s="1">

</xml_diff>

<commit_message>
check for right ip address
</commit_message>
<xml_diff>
--- a/doc/symbols.xlsx
+++ b/doc/symbols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxikrause/VSCode/bambu-mqtt-pico/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45E85A1-8083-DF48-8407-1B22D92C0FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DDD603-BE40-664A-AA67-D2E258CBB3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{03AEDF40-5CD7-D34B-9CD6-B04860BB6D0B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26580" xr2:uid="{03AEDF40-5CD7-D34B-9CD6-B04860BB6D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -111,6 +111,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7B81F8-BA37-E140-A257-454B71F67245}">
-  <dimension ref="D3:AY20"/>
+  <dimension ref="D3:BI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="BL22" sqref="BL22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="1">
         <v>63</v>
       </c>
@@ -576,8 +579,32 @@
       <c r="AY3" s="1">
         <v>56</v>
       </c>
+      <c r="BB3" s="5">
+        <v>63</v>
+      </c>
+      <c r="BC3" s="5">
+        <v>62</v>
+      </c>
+      <c r="BD3" s="5">
+        <v>61</v>
+      </c>
+      <c r="BE3" s="5">
+        <v>60</v>
+      </c>
+      <c r="BF3" s="5">
+        <v>59</v>
+      </c>
+      <c r="BG3" s="5">
+        <v>58</v>
+      </c>
+      <c r="BH3" s="5">
+        <v>57</v>
+      </c>
+      <c r="BI3" s="5">
+        <v>56</v>
+      </c>
     </row>
-    <row r="4" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="1">
         <v>55</v>
       </c>
@@ -698,8 +725,32 @@
       <c r="AY4" s="1">
         <v>48</v>
       </c>
+      <c r="BB4" s="5">
+        <v>55</v>
+      </c>
+      <c r="BC4" s="2">
+        <v>54</v>
+      </c>
+      <c r="BD4" s="5">
+        <v>53</v>
+      </c>
+      <c r="BE4" s="2">
+        <v>52</v>
+      </c>
+      <c r="BF4" s="2">
+        <v>51</v>
+      </c>
+      <c r="BG4" s="2">
+        <v>50</v>
+      </c>
+      <c r="BH4" s="5">
+        <v>49</v>
+      </c>
+      <c r="BI4" s="5">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="1">
         <v>47</v>
       </c>
@@ -820,8 +871,32 @@
       <c r="AY5" s="3">
         <v>40</v>
       </c>
+      <c r="BB5" s="5">
+        <v>47</v>
+      </c>
+      <c r="BC5" s="2">
+        <v>46</v>
+      </c>
+      <c r="BD5" s="5">
+        <v>45</v>
+      </c>
+      <c r="BE5" s="2">
+        <v>44</v>
+      </c>
+      <c r="BF5" s="5">
+        <v>43</v>
+      </c>
+      <c r="BG5" s="2">
+        <v>42</v>
+      </c>
+      <c r="BH5" s="5">
+        <v>41</v>
+      </c>
+      <c r="BI5" s="5">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="1">
         <v>39</v>
       </c>
@@ -942,8 +1017,32 @@
       <c r="AY6" s="1">
         <v>32</v>
       </c>
+      <c r="BB6" s="5">
+        <v>39</v>
+      </c>
+      <c r="BC6" s="2">
+        <v>38</v>
+      </c>
+      <c r="BD6" s="5">
+        <v>37</v>
+      </c>
+      <c r="BE6" s="2">
+        <v>36</v>
+      </c>
+      <c r="BF6" s="2">
+        <v>35</v>
+      </c>
+      <c r="BG6" s="2">
+        <v>34</v>
+      </c>
+      <c r="BH6" s="5">
+        <v>33</v>
+      </c>
+      <c r="BI6" s="5">
+        <v>32</v>
+      </c>
     </row>
-    <row r="7" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="1">
         <v>31</v>
       </c>
@@ -1064,8 +1163,32 @@
       <c r="AY7" s="1">
         <v>24</v>
       </c>
+      <c r="BB7" s="5">
+        <v>31</v>
+      </c>
+      <c r="BC7" s="2">
+        <v>30</v>
+      </c>
+      <c r="BD7" s="5">
+        <v>29</v>
+      </c>
+      <c r="BE7" s="2">
+        <v>28</v>
+      </c>
+      <c r="BF7" s="5">
+        <v>27</v>
+      </c>
+      <c r="BG7" s="5">
+        <v>26</v>
+      </c>
+      <c r="BH7" s="5">
+        <v>25</v>
+      </c>
+      <c r="BI7" s="5">
+        <v>24</v>
+      </c>
     </row>
-    <row r="8" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="1">
         <v>23</v>
       </c>
@@ -1186,8 +1309,32 @@
       <c r="AY8" s="1">
         <v>16</v>
       </c>
+      <c r="BB8" s="5">
+        <v>23</v>
+      </c>
+      <c r="BC8" s="2">
+        <v>22</v>
+      </c>
+      <c r="BD8" s="5">
+        <v>21</v>
+      </c>
+      <c r="BE8" s="2">
+        <v>20</v>
+      </c>
+      <c r="BF8" s="5">
+        <v>19</v>
+      </c>
+      <c r="BG8" s="5">
+        <v>18</v>
+      </c>
+      <c r="BH8" s="5">
+        <v>17</v>
+      </c>
+      <c r="BI8" s="5">
+        <v>16</v>
+      </c>
     </row>
-    <row r="9" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="1">
         <v>15</v>
       </c>
@@ -1308,8 +1455,32 @@
       <c r="AY9" s="1">
         <v>8</v>
       </c>
+      <c r="BB9" s="5">
+        <v>15</v>
+      </c>
+      <c r="BC9" s="2">
+        <v>14</v>
+      </c>
+      <c r="BD9" s="5">
+        <v>13</v>
+      </c>
+      <c r="BE9" s="2">
+        <v>12</v>
+      </c>
+      <c r="BF9" s="5">
+        <v>11</v>
+      </c>
+      <c r="BG9" s="5">
+        <v>10</v>
+      </c>
+      <c r="BH9" s="5">
+        <v>9</v>
+      </c>
+      <c r="BI9" s="5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="1">
         <v>7</v>
       </c>
@@ -1430,8 +1601,32 @@
       <c r="AY10" s="1">
         <v>0</v>
       </c>
+      <c r="BB10" s="5">
+        <v>7</v>
+      </c>
+      <c r="BC10" s="5">
+        <v>6</v>
+      </c>
+      <c r="BD10" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE10" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF10" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG10" s="5">
+        <v>2</v>
+      </c>
+      <c r="BH10" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI10" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D13" s="1">
         <v>63</v>
       </c>
@@ -1552,8 +1747,32 @@
       <c r="AY13" s="1">
         <v>56</v>
       </c>
+      <c r="BB13" s="5">
+        <v>63</v>
+      </c>
+      <c r="BC13" s="5">
+        <v>62</v>
+      </c>
+      <c r="BD13" s="5">
+        <v>61</v>
+      </c>
+      <c r="BE13" s="5">
+        <v>60</v>
+      </c>
+      <c r="BF13" s="5">
+        <v>59</v>
+      </c>
+      <c r="BG13" s="5">
+        <v>58</v>
+      </c>
+      <c r="BH13" s="5">
+        <v>57</v>
+      </c>
+      <c r="BI13" s="5">
+        <v>56</v>
+      </c>
     </row>
-    <row r="14" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="1">
         <v>55</v>
       </c>
@@ -1674,8 +1893,32 @@
       <c r="AY14" s="1">
         <v>48</v>
       </c>
+      <c r="BB14" s="5">
+        <v>55</v>
+      </c>
+      <c r="BC14" s="5">
+        <v>54</v>
+      </c>
+      <c r="BD14" s="2">
+        <v>53</v>
+      </c>
+      <c r="BE14" s="2">
+        <v>52</v>
+      </c>
+      <c r="BF14" s="2">
+        <v>51</v>
+      </c>
+      <c r="BG14" s="5">
+        <v>50</v>
+      </c>
+      <c r="BH14" s="5">
+        <v>49</v>
+      </c>
+      <c r="BI14" s="5">
+        <v>48</v>
+      </c>
     </row>
-    <row r="15" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15" s="1">
         <v>47</v>
       </c>
@@ -1796,8 +2039,32 @@
       <c r="AY15" s="1">
         <v>40</v>
       </c>
+      <c r="BB15" s="5">
+        <v>47</v>
+      </c>
+      <c r="BC15" s="2">
+        <v>46</v>
+      </c>
+      <c r="BD15" s="5">
+        <v>45</v>
+      </c>
+      <c r="BE15" s="5">
+        <v>44</v>
+      </c>
+      <c r="BF15" s="5">
+        <v>43</v>
+      </c>
+      <c r="BG15" s="2">
+        <v>42</v>
+      </c>
+      <c r="BH15" s="5">
+        <v>41</v>
+      </c>
+      <c r="BI15" s="5">
+        <v>40</v>
+      </c>
     </row>
-    <row r="16" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D16" s="1">
         <v>39</v>
       </c>
@@ -1918,8 +2185,32 @@
       <c r="AY16" s="1">
         <v>32</v>
       </c>
+      <c r="BB16" s="5">
+        <v>39</v>
+      </c>
+      <c r="BC16" s="5">
+        <v>38</v>
+      </c>
+      <c r="BD16" s="5">
+        <v>37</v>
+      </c>
+      <c r="BE16" s="5">
+        <v>36</v>
+      </c>
+      <c r="BF16" s="5">
+        <v>35</v>
+      </c>
+      <c r="BG16" s="2">
+        <v>34</v>
+      </c>
+      <c r="BH16" s="5">
+        <v>33</v>
+      </c>
+      <c r="BI16" s="5">
+        <v>32</v>
+      </c>
     </row>
-    <row r="17" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" s="1">
         <v>31</v>
       </c>
@@ -2040,8 +2331,32 @@
       <c r="AY17" s="1">
         <v>24</v>
       </c>
+      <c r="BB17" s="5">
+        <v>31</v>
+      </c>
+      <c r="BC17" s="5">
+        <v>30</v>
+      </c>
+      <c r="BD17" s="5">
+        <v>29</v>
+      </c>
+      <c r="BE17" s="5">
+        <v>28</v>
+      </c>
+      <c r="BF17" s="2">
+        <v>27</v>
+      </c>
+      <c r="BG17" s="5">
+        <v>26</v>
+      </c>
+      <c r="BH17" s="5">
+        <v>25</v>
+      </c>
+      <c r="BI17" s="5">
+        <v>24</v>
+      </c>
     </row>
-    <row r="18" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D18" s="1">
         <v>23</v>
       </c>
@@ -2162,8 +2477,32 @@
       <c r="AY18" s="1">
         <v>16</v>
       </c>
+      <c r="BB18" s="5">
+        <v>23</v>
+      </c>
+      <c r="BC18" s="5">
+        <v>22</v>
+      </c>
+      <c r="BD18" s="5">
+        <v>21</v>
+      </c>
+      <c r="BE18" s="2">
+        <v>20</v>
+      </c>
+      <c r="BF18" s="5">
+        <v>19</v>
+      </c>
+      <c r="BG18" s="5">
+        <v>18</v>
+      </c>
+      <c r="BH18" s="5">
+        <v>17</v>
+      </c>
+      <c r="BI18" s="5">
+        <v>16</v>
+      </c>
     </row>
-    <row r="19" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D19" s="1">
         <v>15</v>
       </c>
@@ -2284,8 +2623,32 @@
       <c r="AY19" s="1">
         <v>8</v>
       </c>
+      <c r="BB19" s="5">
+        <v>15</v>
+      </c>
+      <c r="BC19" s="5">
+        <v>14</v>
+      </c>
+      <c r="BD19" s="5">
+        <v>13</v>
+      </c>
+      <c r="BE19" s="5">
+        <v>12</v>
+      </c>
+      <c r="BF19" s="5">
+        <v>11</v>
+      </c>
+      <c r="BG19" s="5">
+        <v>10</v>
+      </c>
+      <c r="BH19" s="5">
+        <v>9</v>
+      </c>
+      <c r="BI19" s="5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="20" spans="4:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:61" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="1">
         <v>7</v>
       </c>
@@ -2404,6 +2767,30 @@
         <v>1</v>
       </c>
       <c r="AY20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB20" s="5">
+        <v>7</v>
+      </c>
+      <c r="BC20" s="5">
+        <v>6</v>
+      </c>
+      <c r="BD20" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE20" s="2">
+        <v>4</v>
+      </c>
+      <c r="BF20" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG20" s="5">
+        <v>2</v>
+      </c>
+      <c r="BH20" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI20" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>